<commit_message>
update YCL 1 & 2
</commit_message>
<xml_diff>
--- a/Documents/YeuCauLan1/PhanCong.xlsx
+++ b/Documents/YeuCauLan1/PhanCong.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Wind</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>update</t>
   </si>
 </sst>
 </file>
@@ -734,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -940,7 +943,9 @@
       </c>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="F16" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="10" t="s">
         <v>25</v>
@@ -952,7 +957,9 @@
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
+      <c r="F17" s="10" t="s">
+        <v>26</v>
+      </c>
       <c r="G17" s="10"/>
       <c r="H17" s="10" t="s">
         <v>25</v>

</xml_diff>